<commit_message>
Test implementation of connected question (only feedback for now)
</commit_message>
<xml_diff>
--- a/src/data/userdata.xlsx
+++ b/src/data/userdata.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linus\Desktop\NUS\IEX\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FCEED6-0B43-4D1F-AD1D-A93E85F5EB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112687DD-0880-4E58-A380-28F42F741C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="0" windowWidth="27015" windowHeight="14865" activeTab="3" xr2:uid="{01987FBA-0C43-4D57-A1ED-980A623EA11A}"/>
+    <workbookView xWindow="10845" yWindow="495" windowWidth="16515" windowHeight="14865" firstSheet="1" activeTab="4" xr2:uid="{01987FBA-0C43-4D57-A1ED-980A623EA11A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Hetero" sheetId="2" r:id="rId2"/>
     <sheet name="Homo" sheetId="3" r:id="rId3"/>
     <sheet name="Dual test" sheetId="4" r:id="rId4"/>
+    <sheet name="Feedbacktest" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="147">
   <si>
     <t>Gender</t>
   </si>
@@ -600,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -620,6 +621,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6127,8 +6129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B98632-E123-484A-A625-6FE2F1AFB17B}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6443,4 +6445,667 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25208AD9-798C-44FD-861F-F90231C4CD8E}">
+  <dimension ref="A1:O44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>0</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>0</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>0</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M9" s="3">
+        <v>1</v>
+      </c>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3">
+        <v>0.35714286000000001</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3">
+        <v>0</v>
+      </c>
+      <c r="M16" s="3">
+        <v>0</v>
+      </c>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3">
+        <v>1</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0</v>
+      </c>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3">
+        <v>0</v>
+      </c>
+      <c r="M17" s="3">
+        <v>0</v>
+      </c>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>0</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3">
+        <v>3</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3">
+        <v>0</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3">
+        <v>1</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0</v>
+      </c>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>0</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>4</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0</v>
+      </c>
+      <c r="J19" s="3">
+        <v>1</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0</v>
+      </c>
+      <c r="M19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="3">
+        <v>12</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="3">
+        <v>13</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L23" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="D24" s="3">
+        <v>14</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L24" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="D25" s="3">
+        <v>23</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0</v>
+      </c>
+      <c r="L25" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="D26" s="3">
+        <v>24</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0</v>
+      </c>
+      <c r="L26" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="D27" s="3">
+        <v>34</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0</v>
+      </c>
+      <c r="I27" s="3">
+        <v>1</v>
+      </c>
+      <c r="L27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="F30" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="I30" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="L30" s="3">
+        <v>2</v>
+      </c>
+      <c r="M30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>0.25</v>
+      </c>
+      <c r="I33">
+        <v>0.4166666</v>
+      </c>
+      <c r="L33">
+        <v>0.3333333</v>
+      </c>
+    </row>
+    <row r="40" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>0.10714</v>
+      </c>
+      <c r="I40">
+        <v>5.9523E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="H44">
+        <v>0.16666600000000001</v>
+      </c>
+      <c r="L44">
+        <v>0.04</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>